<commit_message>
edited constants, minor additions to payoff new.ipynb
</commit_message>
<xml_diff>
--- a/code/sc/product chart.xlsx
+++ b/code/sc/product chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\NTU Stuff\Y4S1\MH4518 Simulation Techniques in Finance\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\NTU Stuff\Y4S1\MH4518 Simulation Techniques in Finance\Group Project\aaaa\simulation-in-finance\code\sc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCD1A4B-CA1E-49A1-A0B8-6025FA0A5757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFD74C0-B480-4514-B6E0-F9B1767A5266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5508" yWindow="1716" windowWidth="17280" windowHeight="8880" xr2:uid="{6C176C70-7AE9-4030-9E6D-3961EFB80993}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6C176C70-7AE9-4030-9E6D-3961EFB80993}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D82AF4-B2E7-4750-9CF6-A3379B62FE0A}">
   <dimension ref="A1:I479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+    <sheetView tabSelected="1" topLeftCell="A363" workbookViewId="0">
+      <selection activeCell="C379" sqref="C379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +513,7 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <f>NETWORKDAYS($A$2, A2, $I$2:$I$14)</f>
+        <f t="shared" ref="D2:D65" si="0">NETWORKDAYS($A$2, A2, $I$2:$I$15)</f>
         <v>1</v>
       </c>
       <c r="E2">
@@ -532,7 +532,7 @@
         <v>0.97399999999999998</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D66" si="0">NETWORKDAYS($A$2, A3, $I$2:$I$14)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E3">
@@ -648,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="I9" s="1">
-        <v>45380</v>
+        <v>45293</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -670,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="I10" s="1">
-        <v>45383</v>
+        <v>45380</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -686,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="I11" s="1">
-        <v>45413</v>
+        <v>45383</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -702,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="I12" s="1">
-        <v>45421</v>
+        <v>45413</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -721,7 +721,7 @@
         <v>6</v>
       </c>
       <c r="I13" s="1">
-        <v>45432</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -740,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="I14" s="1">
-        <v>45505</v>
+        <v>45432</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -758,6 +758,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="I15" s="1">
+        <v>45505</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -1525,7 +1528,7 @@
         <v>0.96760000000000002</v>
       </c>
       <c r="D66">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D66:D129" si="2">NETWORKDAYS($A$2, A66, $I$2:$I$15)</f>
         <v>44</v>
       </c>
       <c r="E66">
@@ -1538,7 +1541,7 @@
         <v>45108</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D130" si="2">NETWORKDAYS($A$2, A67, $I$2:$I$14)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="E67">
@@ -2495,7 +2498,7 @@
         <v>45171</v>
       </c>
       <c r="D130">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D130:D193" si="4">NETWORKDAYS($A$2, A130, $I$2:$I$15)</f>
         <v>88</v>
       </c>
       <c r="E130">
@@ -2508,7 +2511,7 @@
         <v>45172</v>
       </c>
       <c r="D131">
-        <f t="shared" ref="D131:D194" si="4">NETWORKDAYS($A$2, A131, $I$2:$I$14)</f>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
       <c r="E131">
@@ -3468,7 +3471,7 @@
         <v>45235</v>
       </c>
       <c r="D194">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D194:D257" si="6">NETWORKDAYS($A$2, A194, $I$2:$I$15)</f>
         <v>133</v>
       </c>
       <c r="E194">
@@ -3487,7 +3490,7 @@
         <v>14</v>
       </c>
       <c r="D195">
-        <f t="shared" ref="D195:D258" si="6">NETWORKDAYS($A$2, A195, $I$2:$I$14)</f>
+        <f t="shared" si="6"/>
         <v>134</v>
       </c>
       <c r="E195">
@@ -4244,11 +4247,11 @@
       </c>
       <c r="D252">
         <f t="shared" si="6"/>
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E252">
         <f t="shared" si="7"/>
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.3">
@@ -4257,11 +4260,11 @@
       </c>
       <c r="D253">
         <f t="shared" si="6"/>
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E253">
         <f t="shared" si="7"/>
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
@@ -4270,11 +4273,11 @@
       </c>
       <c r="D254">
         <f t="shared" si="6"/>
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E254">
         <f t="shared" si="7"/>
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
@@ -4283,11 +4286,11 @@
       </c>
       <c r="D255">
         <f t="shared" si="6"/>
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E255">
         <f t="shared" si="7"/>
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
@@ -4296,11 +4299,11 @@
       </c>
       <c r="D256">
         <f t="shared" si="6"/>
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E256">
         <f t="shared" si="7"/>
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
@@ -4309,11 +4312,11 @@
       </c>
       <c r="D257">
         <f t="shared" si="6"/>
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E257">
         <f t="shared" si="7"/>
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.3">
@@ -4321,12 +4324,12 @@
         <v>45299</v>
       </c>
       <c r="D258">
-        <f t="shared" si="6"/>
-        <v>176</v>
+        <f t="shared" ref="D258:D321" si="8">NETWORKDAYS($A$2, A258, $I$2:$I$15)</f>
+        <v>175</v>
       </c>
       <c r="E258">
         <f t="shared" si="7"/>
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.3">
@@ -4334,12 +4337,12 @@
         <v>45300</v>
       </c>
       <c r="D259">
-        <f t="shared" ref="D259:D322" si="8">NETWORKDAYS($A$2, A259, $I$2:$I$14)</f>
-        <v>177</v>
+        <f t="shared" si="8"/>
+        <v>176</v>
       </c>
       <c r="E259">
         <f t="shared" ref="E259:E322" si="9">D259-1</f>
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
@@ -4348,11 +4351,11 @@
       </c>
       <c r="D260">
         <f t="shared" si="8"/>
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E260">
         <f t="shared" si="9"/>
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.3">
@@ -4361,11 +4364,11 @@
       </c>
       <c r="D261">
         <f t="shared" si="8"/>
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E261">
         <f t="shared" si="9"/>
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.3">
@@ -4374,11 +4377,11 @@
       </c>
       <c r="D262">
         <f t="shared" si="8"/>
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E262">
         <f t="shared" si="9"/>
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.3">
@@ -4387,11 +4390,11 @@
       </c>
       <c r="D263">
         <f t="shared" si="8"/>
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E263">
         <f t="shared" si="9"/>
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.3">
@@ -4400,11 +4403,11 @@
       </c>
       <c r="D264">
         <f t="shared" si="8"/>
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E264">
         <f t="shared" si="9"/>
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.3">
@@ -4413,11 +4416,11 @@
       </c>
       <c r="D265">
         <f t="shared" si="8"/>
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E265">
         <f t="shared" si="9"/>
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
@@ -4426,11 +4429,11 @@
       </c>
       <c r="D266">
         <f t="shared" si="8"/>
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E266">
         <f t="shared" si="9"/>
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
@@ -4439,11 +4442,11 @@
       </c>
       <c r="D267">
         <f t="shared" si="8"/>
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E267">
         <f t="shared" si="9"/>
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
@@ -4452,11 +4455,11 @@
       </c>
       <c r="D268">
         <f t="shared" si="8"/>
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E268">
         <f t="shared" si="9"/>
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
@@ -4465,11 +4468,11 @@
       </c>
       <c r="D269">
         <f t="shared" si="8"/>
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E269">
         <f t="shared" si="9"/>
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
@@ -4478,11 +4481,11 @@
       </c>
       <c r="D270">
         <f t="shared" si="8"/>
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E270">
         <f t="shared" si="9"/>
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.3">
@@ -4491,11 +4494,11 @@
       </c>
       <c r="D271">
         <f t="shared" si="8"/>
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E271">
         <f t="shared" si="9"/>
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
@@ -4504,11 +4507,11 @@
       </c>
       <c r="D272">
         <f t="shared" si="8"/>
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E272">
         <f t="shared" si="9"/>
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
@@ -4517,11 +4520,11 @@
       </c>
       <c r="D273">
         <f t="shared" si="8"/>
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E273">
         <f t="shared" si="9"/>
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
@@ -4530,11 +4533,11 @@
       </c>
       <c r="D274">
         <f t="shared" si="8"/>
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E274">
         <f t="shared" si="9"/>
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
@@ -4543,11 +4546,11 @@
       </c>
       <c r="D275">
         <f t="shared" si="8"/>
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E275">
         <f t="shared" si="9"/>
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
@@ -4556,11 +4559,11 @@
       </c>
       <c r="D276">
         <f t="shared" si="8"/>
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E276">
         <f t="shared" si="9"/>
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
@@ -4569,11 +4572,11 @@
       </c>
       <c r="D277">
         <f t="shared" si="8"/>
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E277">
         <f t="shared" si="9"/>
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.3">
@@ -4582,11 +4585,11 @@
       </c>
       <c r="D278">
         <f t="shared" si="8"/>
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E278">
         <f t="shared" si="9"/>
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
@@ -4595,11 +4598,11 @@
       </c>
       <c r="D279">
         <f t="shared" si="8"/>
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E279">
         <f t="shared" si="9"/>
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
@@ -4608,11 +4611,11 @@
       </c>
       <c r="D280">
         <f t="shared" si="8"/>
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E280">
         <f t="shared" si="9"/>
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
@@ -4624,11 +4627,11 @@
       </c>
       <c r="D281">
         <f t="shared" si="8"/>
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E281">
         <f t="shared" si="9"/>
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
@@ -4637,11 +4640,11 @@
       </c>
       <c r="D282">
         <f t="shared" si="8"/>
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E282">
         <f t="shared" si="9"/>
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
@@ -4650,11 +4653,11 @@
       </c>
       <c r="D283">
         <f t="shared" si="8"/>
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E283">
         <f t="shared" si="9"/>
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
@@ -4663,11 +4666,11 @@
       </c>
       <c r="D284">
         <f t="shared" si="8"/>
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E284">
         <f t="shared" si="9"/>
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
@@ -4676,11 +4679,11 @@
       </c>
       <c r="D285">
         <f t="shared" si="8"/>
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E285">
         <f t="shared" si="9"/>
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
@@ -4692,11 +4695,11 @@
       </c>
       <c r="D286">
         <f t="shared" si="8"/>
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E286">
         <f t="shared" si="9"/>
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
@@ -4705,11 +4708,11 @@
       </c>
       <c r="D287">
         <f t="shared" si="8"/>
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E287">
         <f t="shared" si="9"/>
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
@@ -4718,11 +4721,11 @@
       </c>
       <c r="D288">
         <f t="shared" si="8"/>
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E288">
         <f t="shared" si="9"/>
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.3">
@@ -4731,11 +4734,11 @@
       </c>
       <c r="D289">
         <f t="shared" si="8"/>
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E289">
         <f t="shared" si="9"/>
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.3">
@@ -4744,11 +4747,11 @@
       </c>
       <c r="D290">
         <f t="shared" si="8"/>
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E290">
         <f t="shared" si="9"/>
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.3">
@@ -4757,11 +4760,11 @@
       </c>
       <c r="D291">
         <f t="shared" si="8"/>
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E291">
         <f t="shared" si="9"/>
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.3">
@@ -4770,11 +4773,11 @@
       </c>
       <c r="D292">
         <f t="shared" si="8"/>
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E292">
         <f t="shared" si="9"/>
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.3">
@@ -4783,11 +4786,11 @@
       </c>
       <c r="D293">
         <f t="shared" si="8"/>
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E293">
         <f t="shared" si="9"/>
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.3">
@@ -4796,11 +4799,11 @@
       </c>
       <c r="D294">
         <f t="shared" si="8"/>
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E294">
         <f t="shared" si="9"/>
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.3">
@@ -4809,11 +4812,11 @@
       </c>
       <c r="D295">
         <f t="shared" si="8"/>
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E295">
         <f t="shared" si="9"/>
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.3">
@@ -4822,11 +4825,11 @@
       </c>
       <c r="D296">
         <f t="shared" si="8"/>
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E296">
         <f t="shared" si="9"/>
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.3">
@@ -4835,11 +4838,11 @@
       </c>
       <c r="D297">
         <f t="shared" si="8"/>
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E297">
         <f t="shared" si="9"/>
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.3">
@@ -4848,11 +4851,11 @@
       </c>
       <c r="D298">
         <f t="shared" si="8"/>
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E298">
         <f t="shared" si="9"/>
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.3">
@@ -4861,11 +4864,11 @@
       </c>
       <c r="D299">
         <f t="shared" si="8"/>
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E299">
         <f t="shared" si="9"/>
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.3">
@@ -4874,11 +4877,11 @@
       </c>
       <c r="D300">
         <f t="shared" si="8"/>
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E300">
         <f t="shared" si="9"/>
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
@@ -4887,11 +4890,11 @@
       </c>
       <c r="D301">
         <f t="shared" si="8"/>
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E301">
         <f t="shared" si="9"/>
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.3">
@@ -4900,11 +4903,11 @@
       </c>
       <c r="D302">
         <f t="shared" si="8"/>
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E302">
         <f t="shared" si="9"/>
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.3">
@@ -4913,11 +4916,11 @@
       </c>
       <c r="D303">
         <f t="shared" si="8"/>
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E303">
         <f t="shared" si="9"/>
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.3">
@@ -4926,11 +4929,11 @@
       </c>
       <c r="D304">
         <f t="shared" si="8"/>
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E304">
         <f t="shared" si="9"/>
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.3">
@@ -4939,11 +4942,11 @@
       </c>
       <c r="D305">
         <f t="shared" si="8"/>
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E305">
         <f t="shared" si="9"/>
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
@@ -4952,11 +4955,11 @@
       </c>
       <c r="D306">
         <f t="shared" si="8"/>
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E306">
         <f t="shared" si="9"/>
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.3">
@@ -4965,11 +4968,11 @@
       </c>
       <c r="D307">
         <f t="shared" si="8"/>
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E307">
         <f t="shared" si="9"/>
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.3">
@@ -4978,11 +4981,11 @@
       </c>
       <c r="D308">
         <f t="shared" si="8"/>
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E308">
         <f t="shared" si="9"/>
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.3">
@@ -4991,11 +4994,11 @@
       </c>
       <c r="D309">
         <f t="shared" si="8"/>
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E309">
         <f t="shared" si="9"/>
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.3">
@@ -5004,11 +5007,11 @@
       </c>
       <c r="D310">
         <f t="shared" si="8"/>
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E310">
         <f t="shared" si="9"/>
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.3">
@@ -5017,11 +5020,11 @@
       </c>
       <c r="D311">
         <f t="shared" si="8"/>
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E311">
         <f t="shared" si="9"/>
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.3">
@@ -5030,11 +5033,11 @@
       </c>
       <c r="D312">
         <f t="shared" si="8"/>
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E312">
         <f t="shared" si="9"/>
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.3">
@@ -5043,11 +5046,11 @@
       </c>
       <c r="D313">
         <f t="shared" si="8"/>
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E313">
         <f t="shared" si="9"/>
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.3">
@@ -5056,11 +5059,11 @@
       </c>
       <c r="D314">
         <f t="shared" si="8"/>
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E314">
         <f t="shared" si="9"/>
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.3">
@@ -5069,11 +5072,11 @@
       </c>
       <c r="D315">
         <f t="shared" si="8"/>
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E315">
         <f t="shared" si="9"/>
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.3">
@@ -5082,11 +5085,11 @@
       </c>
       <c r="D316">
         <f t="shared" si="8"/>
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E316">
         <f t="shared" si="9"/>
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.3">
@@ -5095,11 +5098,11 @@
       </c>
       <c r="D317">
         <f t="shared" si="8"/>
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E317">
         <f t="shared" si="9"/>
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.3">
@@ -5108,11 +5111,11 @@
       </c>
       <c r="D318">
         <f t="shared" si="8"/>
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E318">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.3">
@@ -5121,11 +5124,11 @@
       </c>
       <c r="D319">
         <f t="shared" si="8"/>
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E319">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.3">
@@ -5134,11 +5137,11 @@
       </c>
       <c r="D320">
         <f t="shared" si="8"/>
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E320">
         <f t="shared" si="9"/>
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.3">
@@ -5147,11 +5150,11 @@
       </c>
       <c r="D321">
         <f t="shared" si="8"/>
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E321">
         <f t="shared" si="9"/>
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.3">
@@ -5159,12 +5162,12 @@
         <v>45363</v>
       </c>
       <c r="D322">
-        <f t="shared" si="8"/>
-        <v>222</v>
+        <f t="shared" ref="D322:D385" si="10">NETWORKDAYS($A$2, A322, $I$2:$I$15)</f>
+        <v>221</v>
       </c>
       <c r="E322">
         <f t="shared" si="9"/>
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.3">
@@ -5172,12 +5175,12 @@
         <v>45364</v>
       </c>
       <c r="D323">
-        <f t="shared" ref="D323:D386" si="10">NETWORKDAYS($A$2, A323, $I$2:$I$14)</f>
-        <v>223</v>
+        <f t="shared" si="10"/>
+        <v>222</v>
       </c>
       <c r="E323">
         <f t="shared" ref="E323:E386" si="11">D323-1</f>
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.3">
@@ -5186,11 +5189,11 @@
       </c>
       <c r="D324">
         <f t="shared" si="10"/>
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E324">
         <f t="shared" si="11"/>
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.3">
@@ -5199,11 +5202,11 @@
       </c>
       <c r="D325">
         <f t="shared" si="10"/>
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E325">
         <f t="shared" si="11"/>
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.3">
@@ -5212,11 +5215,11 @@
       </c>
       <c r="D326">
         <f t="shared" si="10"/>
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E326">
         <f t="shared" si="11"/>
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.3">
@@ -5225,11 +5228,11 @@
       </c>
       <c r="D327">
         <f t="shared" si="10"/>
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E327">
         <f t="shared" si="11"/>
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.3">
@@ -5238,11 +5241,11 @@
       </c>
       <c r="D328">
         <f t="shared" si="10"/>
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E328">
         <f t="shared" si="11"/>
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.3">
@@ -5251,11 +5254,11 @@
       </c>
       <c r="D329">
         <f t="shared" si="10"/>
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E329">
         <f t="shared" si="11"/>
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.3">
@@ -5264,11 +5267,11 @@
       </c>
       <c r="D330">
         <f t="shared" si="10"/>
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E330">
         <f t="shared" si="11"/>
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.3">
@@ -5277,11 +5280,11 @@
       </c>
       <c r="D331">
         <f t="shared" si="10"/>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E331">
         <f t="shared" si="11"/>
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.3">
@@ -5290,11 +5293,11 @@
       </c>
       <c r="D332">
         <f t="shared" si="10"/>
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E332">
         <f t="shared" si="11"/>
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.3">
@@ -5303,11 +5306,11 @@
       </c>
       <c r="D333">
         <f t="shared" si="10"/>
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E333">
         <f t="shared" si="11"/>
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.3">
@@ -5316,11 +5319,11 @@
       </c>
       <c r="D334">
         <f t="shared" si="10"/>
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E334">
         <f t="shared" si="11"/>
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.3">
@@ -5329,11 +5332,11 @@
       </c>
       <c r="D335">
         <f t="shared" si="10"/>
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E335">
         <f t="shared" si="11"/>
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.3">
@@ -5342,11 +5345,11 @@
       </c>
       <c r="D336">
         <f t="shared" si="10"/>
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E336">
         <f t="shared" si="11"/>
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.3">
@@ -5355,11 +5358,11 @@
       </c>
       <c r="D337">
         <f t="shared" si="10"/>
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E337">
         <f t="shared" si="11"/>
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.3">
@@ -5368,11 +5371,11 @@
       </c>
       <c r="D338">
         <f t="shared" si="10"/>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E338">
         <f t="shared" si="11"/>
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.3">
@@ -5384,11 +5387,11 @@
       </c>
       <c r="D339">
         <f t="shared" si="10"/>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E339">
         <f t="shared" si="11"/>
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.3">
@@ -5397,11 +5400,11 @@
       </c>
       <c r="D340">
         <f t="shared" si="10"/>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E340">
         <f t="shared" si="11"/>
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.3">
@@ -5410,11 +5413,11 @@
       </c>
       <c r="D341">
         <f t="shared" si="10"/>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E341">
         <f t="shared" si="11"/>
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.3">
@@ -5426,11 +5429,11 @@
       </c>
       <c r="D342">
         <f t="shared" si="10"/>
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E342">
         <f t="shared" si="11"/>
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.3">
@@ -5439,11 +5442,11 @@
       </c>
       <c r="D343">
         <f t="shared" si="10"/>
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E343">
         <f t="shared" si="11"/>
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.3">
@@ -5452,11 +5455,11 @@
       </c>
       <c r="D344">
         <f t="shared" si="10"/>
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E344">
         <f t="shared" si="11"/>
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.3">
@@ -5465,11 +5468,11 @@
       </c>
       <c r="D345">
         <f t="shared" si="10"/>
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E345">
         <f t="shared" si="11"/>
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.3">
@@ -5478,11 +5481,11 @@
       </c>
       <c r="D346">
         <f t="shared" si="10"/>
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E346">
         <f t="shared" si="11"/>
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.3">
@@ -5491,11 +5494,11 @@
       </c>
       <c r="D347">
         <f t="shared" si="10"/>
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E347">
         <f t="shared" si="11"/>
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.3">
@@ -5504,11 +5507,11 @@
       </c>
       <c r="D348">
         <f t="shared" si="10"/>
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E348">
         <f t="shared" si="11"/>
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.3">
@@ -5517,11 +5520,11 @@
       </c>
       <c r="D349">
         <f t="shared" si="10"/>
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E349">
         <f t="shared" si="11"/>
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.3">
@@ -5530,11 +5533,11 @@
       </c>
       <c r="D350">
         <f t="shared" si="10"/>
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E350">
         <f t="shared" si="11"/>
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.3">
@@ -5543,11 +5546,11 @@
       </c>
       <c r="D351">
         <f t="shared" si="10"/>
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E351">
         <f t="shared" si="11"/>
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.3">
@@ -5556,11 +5559,11 @@
       </c>
       <c r="D352">
         <f t="shared" si="10"/>
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E352">
         <f t="shared" si="11"/>
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.3">
@@ -5569,11 +5572,11 @@
       </c>
       <c r="D353">
         <f t="shared" si="10"/>
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E353">
         <f t="shared" si="11"/>
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.3">
@@ -5582,11 +5585,11 @@
       </c>
       <c r="D354">
         <f t="shared" si="10"/>
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E354">
         <f t="shared" si="11"/>
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.3">
@@ -5595,11 +5598,11 @@
       </c>
       <c r="D355">
         <f t="shared" si="10"/>
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E355">
         <f t="shared" si="11"/>
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.3">
@@ -5608,11 +5611,11 @@
       </c>
       <c r="D356">
         <f t="shared" si="10"/>
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E356">
         <f t="shared" si="11"/>
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.3">
@@ -5621,11 +5624,11 @@
       </c>
       <c r="D357">
         <f t="shared" si="10"/>
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E357">
         <f t="shared" si="11"/>
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.3">
@@ -5634,11 +5637,11 @@
       </c>
       <c r="D358">
         <f t="shared" si="10"/>
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E358">
         <f t="shared" si="11"/>
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.3">
@@ -5647,11 +5650,11 @@
       </c>
       <c r="D359">
         <f t="shared" si="10"/>
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E359">
         <f t="shared" si="11"/>
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.3">
@@ -5660,11 +5663,11 @@
       </c>
       <c r="D360">
         <f t="shared" si="10"/>
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E360">
         <f t="shared" si="11"/>
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.3">
@@ -5673,11 +5676,11 @@
       </c>
       <c r="D361">
         <f t="shared" si="10"/>
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E361">
         <f t="shared" si="11"/>
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.3">
@@ -5686,11 +5689,11 @@
       </c>
       <c r="D362">
         <f t="shared" si="10"/>
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E362">
         <f t="shared" si="11"/>
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.3">
@@ -5699,11 +5702,11 @@
       </c>
       <c r="D363">
         <f t="shared" si="10"/>
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E363">
         <f t="shared" si="11"/>
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.3">
@@ -5712,11 +5715,11 @@
       </c>
       <c r="D364">
         <f t="shared" si="10"/>
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E364">
         <f t="shared" si="11"/>
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.3">
@@ -5725,11 +5728,11 @@
       </c>
       <c r="D365">
         <f t="shared" si="10"/>
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E365">
         <f t="shared" si="11"/>
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.3">
@@ -5738,11 +5741,11 @@
       </c>
       <c r="D366">
         <f t="shared" si="10"/>
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E366">
         <f t="shared" si="11"/>
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.3">
@@ -5751,11 +5754,11 @@
       </c>
       <c r="D367">
         <f t="shared" si="10"/>
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E367">
         <f t="shared" si="11"/>
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.3">
@@ -5764,11 +5767,11 @@
       </c>
       <c r="D368">
         <f t="shared" si="10"/>
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E368">
         <f t="shared" si="11"/>
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.3">
@@ -5777,11 +5780,11 @@
       </c>
       <c r="D369">
         <f t="shared" si="10"/>
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E369">
         <f t="shared" si="11"/>
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.3">
@@ -5790,11 +5793,11 @@
       </c>
       <c r="D370">
         <f t="shared" si="10"/>
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E370">
         <f t="shared" si="11"/>
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.3">
@@ -5806,11 +5809,11 @@
       </c>
       <c r="D371">
         <f t="shared" si="10"/>
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E371">
         <f t="shared" si="11"/>
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.3">
@@ -5822,11 +5825,11 @@
       </c>
       <c r="D372">
         <f t="shared" si="10"/>
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E372">
         <f t="shared" si="11"/>
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.3">
@@ -5835,11 +5838,11 @@
       </c>
       <c r="D373">
         <f t="shared" si="10"/>
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E373">
         <f t="shared" si="11"/>
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.3">
@@ -5848,11 +5851,11 @@
       </c>
       <c r="D374">
         <f t="shared" si="10"/>
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E374">
         <f t="shared" si="11"/>
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.3">
@@ -5861,11 +5864,11 @@
       </c>
       <c r="D375">
         <f t="shared" si="10"/>
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E375">
         <f t="shared" si="11"/>
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.3">
@@ -5874,11 +5877,11 @@
       </c>
       <c r="D376">
         <f t="shared" si="10"/>
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E376">
         <f t="shared" si="11"/>
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.3">
@@ -5890,11 +5893,11 @@
       </c>
       <c r="D377">
         <f t="shared" si="10"/>
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E377">
         <f t="shared" si="11"/>
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.3">
@@ -5903,11 +5906,11 @@
       </c>
       <c r="D378">
         <f t="shared" si="10"/>
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E378">
         <f t="shared" si="11"/>
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.3">
@@ -5916,11 +5919,11 @@
       </c>
       <c r="D379">
         <f t="shared" si="10"/>
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E379">
         <f t="shared" si="11"/>
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.3">
@@ -5932,11 +5935,11 @@
       </c>
       <c r="D380">
         <f t="shared" si="10"/>
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E380">
         <f t="shared" si="11"/>
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.3">
@@ -5945,11 +5948,11 @@
       </c>
       <c r="D381">
         <f t="shared" si="10"/>
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E381">
         <f t="shared" si="11"/>
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.3">
@@ -5958,11 +5961,11 @@
       </c>
       <c r="D382">
         <f t="shared" si="10"/>
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E382">
         <f t="shared" si="11"/>
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.3">
@@ -5971,11 +5974,11 @@
       </c>
       <c r="D383">
         <f t="shared" si="10"/>
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E383">
         <f t="shared" si="11"/>
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.3">
@@ -5984,11 +5987,11 @@
       </c>
       <c r="D384">
         <f t="shared" si="10"/>
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E384">
         <f t="shared" si="11"/>
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.3">
@@ -5997,11 +6000,11 @@
       </c>
       <c r="D385">
         <f t="shared" si="10"/>
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E385">
         <f t="shared" si="11"/>
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.3">
@@ -6009,12 +6012,12 @@
         <v>45427</v>
       </c>
       <c r="D386">
-        <f t="shared" si="10"/>
-        <v>264</v>
+        <f t="shared" ref="D386:D449" si="12">NETWORKDAYS($A$2, A386, $I$2:$I$15)</f>
+        <v>263</v>
       </c>
       <c r="E386">
         <f t="shared" si="11"/>
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.3">
@@ -6022,12 +6025,12 @@
         <v>45428</v>
       </c>
       <c r="D387">
-        <f t="shared" ref="D387:D450" si="12">NETWORKDAYS($A$2, A387, $I$2:$I$14)</f>
-        <v>265</v>
+        <f t="shared" si="12"/>
+        <v>264</v>
       </c>
       <c r="E387">
         <f t="shared" ref="E387:E450" si="13">D387-1</f>
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.3">
@@ -6036,11 +6039,11 @@
       </c>
       <c r="D388">
         <f t="shared" si="12"/>
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E388">
         <f t="shared" si="13"/>
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.3">
@@ -6049,11 +6052,11 @@
       </c>
       <c r="D389">
         <f t="shared" si="12"/>
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E389">
         <f t="shared" si="13"/>
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.3">
@@ -6062,11 +6065,11 @@
       </c>
       <c r="D390">
         <f t="shared" si="12"/>
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E390">
         <f t="shared" si="13"/>
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.3">
@@ -6078,11 +6081,11 @@
       </c>
       <c r="D391">
         <f t="shared" si="12"/>
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E391">
         <f t="shared" si="13"/>
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.3">
@@ -6091,11 +6094,11 @@
       </c>
       <c r="D392">
         <f t="shared" si="12"/>
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E392">
         <f t="shared" si="13"/>
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.3">
@@ -6104,11 +6107,11 @@
       </c>
       <c r="D393">
         <f t="shared" si="12"/>
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E393">
         <f t="shared" si="13"/>
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.3">
@@ -6117,11 +6120,11 @@
       </c>
       <c r="D394">
         <f t="shared" si="12"/>
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E394">
         <f t="shared" si="13"/>
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.3">
@@ -6130,11 +6133,11 @@
       </c>
       <c r="D395">
         <f t="shared" si="12"/>
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E395">
         <f t="shared" si="13"/>
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.3">
@@ -6143,11 +6146,11 @@
       </c>
       <c r="D396">
         <f t="shared" si="12"/>
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E396">
         <f t="shared" si="13"/>
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.3">
@@ -6156,11 +6159,11 @@
       </c>
       <c r="D397">
         <f t="shared" si="12"/>
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E397">
         <f t="shared" si="13"/>
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.3">
@@ -6169,11 +6172,11 @@
       </c>
       <c r="D398">
         <f t="shared" si="12"/>
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E398">
         <f t="shared" si="13"/>
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.3">
@@ -6182,11 +6185,11 @@
       </c>
       <c r="D399">
         <f t="shared" si="12"/>
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E399">
         <f t="shared" si="13"/>
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.3">
@@ -6195,11 +6198,11 @@
       </c>
       <c r="D400">
         <f t="shared" si="12"/>
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E400">
         <f t="shared" si="13"/>
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.3">
@@ -6208,11 +6211,11 @@
       </c>
       <c r="D401">
         <f t="shared" si="12"/>
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E401">
         <f t="shared" si="13"/>
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.3">
@@ -6221,11 +6224,11 @@
       </c>
       <c r="D402">
         <f t="shared" si="12"/>
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E402">
         <f t="shared" si="13"/>
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.3">
@@ -6234,11 +6237,11 @@
       </c>
       <c r="D403">
         <f t="shared" si="12"/>
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E403">
         <f t="shared" si="13"/>
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.3">
@@ -6247,11 +6250,11 @@
       </c>
       <c r="D404">
         <f t="shared" si="12"/>
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E404">
         <f t="shared" si="13"/>
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.3">
@@ -6260,11 +6263,11 @@
       </c>
       <c r="D405">
         <f t="shared" si="12"/>
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E405">
         <f t="shared" si="13"/>
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.3">
@@ -6273,11 +6276,11 @@
       </c>
       <c r="D406">
         <f t="shared" si="12"/>
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E406">
         <f t="shared" si="13"/>
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.3">
@@ -6286,11 +6289,11 @@
       </c>
       <c r="D407">
         <f t="shared" si="12"/>
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E407">
         <f t="shared" si="13"/>
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.3">
@@ -6299,11 +6302,11 @@
       </c>
       <c r="D408">
         <f t="shared" si="12"/>
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E408">
         <f t="shared" si="13"/>
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.3">
@@ -6312,11 +6315,11 @@
       </c>
       <c r="D409">
         <f t="shared" si="12"/>
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E409">
         <f t="shared" si="13"/>
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.3">
@@ -6325,11 +6328,11 @@
       </c>
       <c r="D410">
         <f t="shared" si="12"/>
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E410">
         <f t="shared" si="13"/>
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.3">
@@ -6338,11 +6341,11 @@
       </c>
       <c r="D411">
         <f t="shared" si="12"/>
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E411">
         <f t="shared" si="13"/>
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.3">
@@ -6351,11 +6354,11 @@
       </c>
       <c r="D412">
         <f t="shared" si="12"/>
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E412">
         <f t="shared" si="13"/>
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.3">
@@ -6364,11 +6367,11 @@
       </c>
       <c r="D413">
         <f t="shared" si="12"/>
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E413">
         <f t="shared" si="13"/>
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.3">
@@ -6377,11 +6380,11 @@
       </c>
       <c r="D414">
         <f t="shared" si="12"/>
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E414">
         <f t="shared" si="13"/>
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.3">
@@ -6390,11 +6393,11 @@
       </c>
       <c r="D415">
         <f t="shared" si="12"/>
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E415">
         <f t="shared" si="13"/>
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.3">
@@ -6403,11 +6406,11 @@
       </c>
       <c r="D416">
         <f t="shared" si="12"/>
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E416">
         <f t="shared" si="13"/>
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.3">
@@ -6416,11 +6419,11 @@
       </c>
       <c r="D417">
         <f t="shared" si="12"/>
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E417">
         <f t="shared" si="13"/>
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.3">
@@ -6429,11 +6432,11 @@
       </c>
       <c r="D418">
         <f t="shared" si="12"/>
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E418">
         <f t="shared" si="13"/>
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.3">
@@ -6442,11 +6445,11 @@
       </c>
       <c r="D419">
         <f t="shared" si="12"/>
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E419">
         <f t="shared" si="13"/>
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.3">
@@ -6455,11 +6458,11 @@
       </c>
       <c r="D420">
         <f t="shared" si="12"/>
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E420">
         <f t="shared" si="13"/>
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.3">
@@ -6468,11 +6471,11 @@
       </c>
       <c r="D421">
         <f t="shared" si="12"/>
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E421">
         <f t="shared" si="13"/>
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.3">
@@ -6481,11 +6484,11 @@
       </c>
       <c r="D422">
         <f t="shared" si="12"/>
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E422">
         <f t="shared" si="13"/>
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.3">
@@ -6494,11 +6497,11 @@
       </c>
       <c r="D423">
         <f t="shared" si="12"/>
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E423">
         <f t="shared" si="13"/>
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.3">
@@ -6507,11 +6510,11 @@
       </c>
       <c r="D424">
         <f t="shared" si="12"/>
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E424">
         <f t="shared" si="13"/>
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.3">
@@ -6520,11 +6523,11 @@
       </c>
       <c r="D425">
         <f t="shared" si="12"/>
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E425">
         <f t="shared" si="13"/>
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.3">
@@ -6533,11 +6536,11 @@
       </c>
       <c r="D426">
         <f t="shared" si="12"/>
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E426">
         <f t="shared" si="13"/>
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.3">
@@ -6546,11 +6549,11 @@
       </c>
       <c r="D427">
         <f t="shared" si="12"/>
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E427">
         <f t="shared" si="13"/>
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.3">
@@ -6559,11 +6562,11 @@
       </c>
       <c r="D428">
         <f t="shared" si="12"/>
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E428">
         <f t="shared" si="13"/>
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.3">
@@ -6572,11 +6575,11 @@
       </c>
       <c r="D429">
         <f t="shared" si="12"/>
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E429">
         <f t="shared" si="13"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.3">
@@ -6585,11 +6588,11 @@
       </c>
       <c r="D430">
         <f t="shared" si="12"/>
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E430">
         <f t="shared" si="13"/>
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.3">
@@ -6598,11 +6601,11 @@
       </c>
       <c r="D431">
         <f t="shared" si="12"/>
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E431">
         <f t="shared" si="13"/>
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.3">
@@ -6611,11 +6614,11 @@
       </c>
       <c r="D432">
         <f t="shared" si="12"/>
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E432">
         <f t="shared" si="13"/>
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.3">
@@ -6624,11 +6627,11 @@
       </c>
       <c r="D433">
         <f t="shared" si="12"/>
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E433">
         <f t="shared" si="13"/>
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.3">
@@ -6637,11 +6640,11 @@
       </c>
       <c r="D434">
         <f t="shared" si="12"/>
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E434">
         <f t="shared" si="13"/>
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.3">
@@ -6650,11 +6653,11 @@
       </c>
       <c r="D435">
         <f t="shared" si="12"/>
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E435">
         <f t="shared" si="13"/>
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.3">
@@ -6663,11 +6666,11 @@
       </c>
       <c r="D436">
         <f t="shared" si="12"/>
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E436">
         <f t="shared" si="13"/>
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.3">
@@ -6676,11 +6679,11 @@
       </c>
       <c r="D437">
         <f t="shared" si="12"/>
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E437">
         <f t="shared" si="13"/>
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.3">
@@ -6689,11 +6692,11 @@
       </c>
       <c r="D438">
         <f t="shared" si="12"/>
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E438">
         <f t="shared" si="13"/>
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.3">
@@ -6702,11 +6705,11 @@
       </c>
       <c r="D439">
         <f t="shared" si="12"/>
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E439">
         <f t="shared" si="13"/>
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.3">
@@ -6715,11 +6718,11 @@
       </c>
       <c r="D440">
         <f t="shared" si="12"/>
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E440">
         <f t="shared" si="13"/>
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.3">
@@ -6728,11 +6731,11 @@
       </c>
       <c r="D441">
         <f t="shared" si="12"/>
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E441">
         <f t="shared" si="13"/>
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.3">
@@ -6741,11 +6744,11 @@
       </c>
       <c r="D442">
         <f t="shared" si="12"/>
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E442">
         <f t="shared" si="13"/>
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.3">
@@ -6754,11 +6757,11 @@
       </c>
       <c r="D443">
         <f t="shared" si="12"/>
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E443">
         <f t="shared" si="13"/>
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.3">
@@ -6767,11 +6770,11 @@
       </c>
       <c r="D444">
         <f t="shared" si="12"/>
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E444">
         <f t="shared" si="13"/>
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.3">
@@ -6780,11 +6783,11 @@
       </c>
       <c r="D445">
         <f t="shared" si="12"/>
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E445">
         <f t="shared" si="13"/>
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.3">
@@ -6793,11 +6796,11 @@
       </c>
       <c r="D446">
         <f t="shared" si="12"/>
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E446">
         <f t="shared" si="13"/>
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.3">
@@ -6806,11 +6809,11 @@
       </c>
       <c r="D447">
         <f t="shared" si="12"/>
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E447">
         <f t="shared" si="13"/>
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.3">
@@ -6819,11 +6822,11 @@
       </c>
       <c r="D448">
         <f t="shared" si="12"/>
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E448">
         <f t="shared" si="13"/>
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.3">
@@ -6832,11 +6835,11 @@
       </c>
       <c r="D449">
         <f t="shared" si="12"/>
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E449">
         <f t="shared" si="13"/>
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.3">
@@ -6844,12 +6847,12 @@
         <v>45491</v>
       </c>
       <c r="D450">
-        <f t="shared" si="12"/>
-        <v>309</v>
+        <f t="shared" ref="D450:D479" si="14">NETWORKDAYS($A$2, A450, $I$2:$I$15)</f>
+        <v>308</v>
       </c>
       <c r="E450">
         <f t="shared" si="13"/>
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.3">
@@ -6857,12 +6860,12 @@
         <v>45492</v>
       </c>
       <c r="D451">
-        <f t="shared" ref="D451:D479" si="14">NETWORKDAYS($A$2, A451, $I$2:$I$14)</f>
-        <v>310</v>
+        <f t="shared" si="14"/>
+        <v>309</v>
       </c>
       <c r="E451">
         <f t="shared" ref="E451:E479" si="15">D451-1</f>
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.3">
@@ -6871,11 +6874,11 @@
       </c>
       <c r="D452">
         <f t="shared" si="14"/>
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E452">
         <f t="shared" si="15"/>
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.3">
@@ -6884,11 +6887,11 @@
       </c>
       <c r="D453">
         <f t="shared" si="14"/>
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E453">
         <f t="shared" si="15"/>
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.3">
@@ -6897,11 +6900,11 @@
       </c>
       <c r="D454">
         <f t="shared" si="14"/>
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E454">
         <f t="shared" si="15"/>
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.3">
@@ -6910,11 +6913,11 @@
       </c>
       <c r="D455">
         <f t="shared" si="14"/>
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E455">
         <f t="shared" si="15"/>
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.3">
@@ -6923,11 +6926,11 @@
       </c>
       <c r="D456">
         <f t="shared" si="14"/>
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E456">
         <f t="shared" si="15"/>
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.3">
@@ -6936,11 +6939,11 @@
       </c>
       <c r="D457">
         <f t="shared" si="14"/>
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E457">
         <f t="shared" si="15"/>
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.3">
@@ -6949,11 +6952,11 @@
       </c>
       <c r="D458">
         <f t="shared" si="14"/>
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E458">
         <f t="shared" si="15"/>
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.3">
@@ -6962,11 +6965,11 @@
       </c>
       <c r="D459">
         <f t="shared" si="14"/>
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E459">
         <f t="shared" si="15"/>
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.3">
@@ -6975,11 +6978,11 @@
       </c>
       <c r="D460">
         <f t="shared" si="14"/>
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E460">
         <f t="shared" si="15"/>
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.3">
@@ -6988,11 +6991,11 @@
       </c>
       <c r="D461">
         <f t="shared" si="14"/>
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E461">
         <f t="shared" si="15"/>
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.3">
@@ -7004,11 +7007,11 @@
       </c>
       <c r="D462">
         <f t="shared" si="14"/>
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E462">
         <f t="shared" si="15"/>
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.3">
@@ -7017,11 +7020,11 @@
       </c>
       <c r="D463">
         <f t="shared" si="14"/>
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E463">
         <f t="shared" si="15"/>
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.3">
@@ -7033,11 +7036,11 @@
       </c>
       <c r="D464">
         <f t="shared" si="14"/>
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E464">
         <f t="shared" si="15"/>
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.3">
@@ -7046,11 +7049,11 @@
       </c>
       <c r="D465">
         <f t="shared" si="14"/>
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E465">
         <f t="shared" si="15"/>
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.3">
@@ -7059,11 +7062,11 @@
       </c>
       <c r="D466">
         <f t="shared" si="14"/>
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E466">
         <f t="shared" si="15"/>
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.3">
@@ -7072,11 +7075,11 @@
       </c>
       <c r="D467">
         <f t="shared" si="14"/>
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E467">
         <f t="shared" si="15"/>
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.3">
@@ -7088,11 +7091,11 @@
       </c>
       <c r="D468">
         <f t="shared" si="14"/>
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E468">
         <f t="shared" si="15"/>
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.3">
@@ -7101,11 +7104,11 @@
       </c>
       <c r="D469">
         <f t="shared" si="14"/>
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E469">
         <f t="shared" si="15"/>
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.3">
@@ -7114,11 +7117,11 @@
       </c>
       <c r="D470">
         <f t="shared" si="14"/>
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E470">
         <f t="shared" si="15"/>
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.3">
@@ -7127,11 +7130,11 @@
       </c>
       <c r="D471">
         <f t="shared" si="14"/>
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E471">
         <f t="shared" si="15"/>
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.3">
@@ -7140,11 +7143,11 @@
       </c>
       <c r="D472">
         <f t="shared" si="14"/>
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E472">
         <f t="shared" si="15"/>
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.3">
@@ -7153,11 +7156,11 @@
       </c>
       <c r="D473">
         <f t="shared" si="14"/>
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E473">
         <f t="shared" si="15"/>
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.3">
@@ -7166,11 +7169,11 @@
       </c>
       <c r="D474">
         <f t="shared" si="14"/>
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E474">
         <f t="shared" si="15"/>
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.3">
@@ -7179,11 +7182,11 @@
       </c>
       <c r="D475">
         <f t="shared" si="14"/>
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E475">
         <f t="shared" si="15"/>
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.3">
@@ -7192,11 +7195,11 @@
       </c>
       <c r="D476">
         <f t="shared" si="14"/>
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E476">
         <f t="shared" si="15"/>
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.3">
@@ -7205,11 +7208,11 @@
       </c>
       <c r="D477">
         <f t="shared" si="14"/>
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E477">
         <f t="shared" si="15"/>
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.3">
@@ -7218,11 +7221,11 @@
       </c>
       <c r="D478">
         <f t="shared" si="14"/>
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E478">
         <f t="shared" si="15"/>
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.3">
@@ -7231,11 +7234,11 @@
       </c>
       <c r="D479">
         <f t="shared" si="14"/>
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E479">
         <f t="shared" si="15"/>
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>